<commit_message>
Fixed issues in .xlsx file.
</commit_message>
<xml_diff>
--- a/spreadsheets/xlookup-complete-tutorial/xlookup-complete-tutorial.xlsx
+++ b/spreadsheets/xlookup-complete-tutorial/xlookup-complete-tutorial.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Content\Microsoft Excel\XLOOKUP\00001 - Tutorial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Content\my-content\Microsoft Excel\XLOOKUP\00001 - Tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8165E34F-C5E8-4717-80C2-9A6304670497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF969D9-2D4C-4EEB-97D6-4664A4A7997E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="E1 - Vertical Lookup" sheetId="14" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="193">
   <si>
     <t>Country</t>
   </si>
@@ -678,12 +678,6 @@
   </si>
   <si>
     <t>South Sudan</t>
-  </si>
-  <si>
-    <t>Hapiness Score</t>
-  </si>
-  <si>
-    <t>Hapiness Rank</t>
   </si>
   <si>
     <t>Economy (GDP per Capita Rounded)</t>
@@ -1439,7 +1433,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B20"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1502,7 +1496,7 @@
       <c r="H2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="2">
         <f>_xlfn.XLOOKUP(H2,A2:A20,D2:D20)</f>
         <v>6.9370000000000003</v>
       </c>
@@ -8388,7 +8382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22B2875F-ABC1-4392-AFB0-2B3FFC4A0EF5}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -8518,7 +8512,7 @@
     <col min="5" max="5" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -8544,7 +8538,7 @@
         <v>0</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -8570,7 +8564,7 @@
         <v>37</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f>_xlfn.XLOOKUP(H2, A2:A20, B2:B20, "Country not found")</f>
+        <f>_xlfn.XLOOKUP(H2, A2:A20, D2:D20, "Country not found")</f>
         <v>Country not found</v>
       </c>
     </row>
@@ -8946,7 +8940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5C5ABD-6B6E-4246-A9F5-C271F3692FE2}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -8982,7 +8976,7 @@
         <v>7</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>188</v>
+        <v>3</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>0</v>
@@ -9449,11 +9443,11 @@
         <v>0.94142999999999999</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="I2" s="2" t="str">
         <f>_xlfn.XLOOKUP(H2, B2:B20, A2:A20, "Region not found", 1, -1)</f>
-        <v>United States</v>
+        <v>Brazil</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -9829,7 +9823,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9871,7 +9865,7 @@
         <v>1</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>189</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -9923,6 +9917,10 @@
       <c r="F3">
         <v>0.94784000000000002</v>
       </c>
+      <c r="I3" t="str" cm="1">
+        <f t="array" ref="I3">_xlfn.XLOOKUP(H2, A2:A20,B2:B20&amp;C2:C20)</f>
+        <v>Western Europe2</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -9942,6 +9940,10 @@
       </c>
       <c r="F4">
         <v>0.87463999999999997</v>
+      </c>
+      <c r="I4" t="str" cm="1">
+        <f t="array" ref="I4">_xlfn.XLOOKUP(H2, A2:A20,B2:B20&amp;", "&amp;C2:C20)</f>
+        <v>Western Europe, 2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -10277,7 +10279,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10307,7 +10309,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -10319,7 +10321,7 @@
         <v>1</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>0</v>
@@ -10784,7 +10786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB359CD-E5E4-444B-A02E-8A253A583F1B}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -10820,13 +10822,13 @@
         <v>7</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>